<commit_message>
project update version 63493
</commit_message>
<xml_diff>
--- a/lib/vendor/phpoffice/phpspreadsheet/samples/templates/32readwriteStockChart2.xlsx
+++ b/lib/vendor/phpoffice/phpspreadsheet/samples/templates/32readwriteStockChart2.xlsx
@@ -1,16 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\stockchart\samples\templates\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6651DBCB-E908-4572-89E5-32CA2D395A02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="96" windowWidth="20736" windowHeight="11760" activeTab="1"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
     <sheet name="Charts" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -62,7 +81,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -131,14 +150,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -262,6 +284,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-EC95-49B5-9C61-114DD1FD4579}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -369,6 +396,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-EC95-49B5-9C61-114DD1FD4579}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -476,6 +508,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-EC95-49B5-9C61-114DD1FD4579}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -496,6 +533,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -540,9 +578,9 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -569,7 +607,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -662,45 +699,50 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>130</c:v>
+                  <c:v>147</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>132</c:v>
+                  <c:v>146</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>125</c:v>
+                  <c:v>206</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>141</c:v>
+                  <c:v>215</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>156</c:v>
+                  <c:v>262</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>215</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>193</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>159</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>194</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>154</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>148</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>182</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>170</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>173</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>163</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>271</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>276</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-53E9-47AC-A9DD-55E40E59CF26}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="0"/>
@@ -791,42 +833,47 @@
                   <c:v>204</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>197</c:v>
+                  <c:v>211</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>186</c:v>
+                  <c:v>314</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>177</c:v>
+                  <c:v>283</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>211</c:v>
+                  <c:v>358</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>195</c:v>
+                  <c:v>262</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>223</c:v>
+                  <c:v>295</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>275</c:v>
+                  <c:v>232</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>279</c:v>
+                  <c:v>226</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>271</c:v>
+                  <c:v>264</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>310</c:v>
+                  <c:v>180</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>305</c:v>
+                  <c:v>208</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-53E9-47AC-A9DD-55E40E59CF26}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -914,45 +961,50 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>109</c:v>
+                  <c:v>116</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>85</c:v>
+                  <c:v>121</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>87</c:v>
+                  <c:v>162</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>108</c:v>
+                  <c:v>194</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>134</c:v>
+                  <c:v>214</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>124</c:v>
+                  <c:v>192</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>146</c:v>
+                  <c:v>149</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>130</c:v>
+                  <c:v>131</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>127</c:v>
+                  <c:v>173</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>131</c:v>
+                  <c:v>148</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>249</c:v>
+                  <c:v>122</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>241</c:v>
+                  <c:v>118</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-53E9-47AC-A9DD-55E40E59CF26}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
@@ -1040,45 +1092,50 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>132</c:v>
+                  <c:v>146</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>125</c:v>
+                  <c:v>206</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>141</c:v>
+                  <c:v>215</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>156</c:v>
+                  <c:v>262</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>215</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>193</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>159</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>194</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>154</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>148</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>182</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>170</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>173</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>163</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>271</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>276</c:v>
-                </c:pt>
                 <c:pt idx="11">
-                  <c:v>245</c:v>
+                  <c:v>165</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-53E9-47AC-A9DD-55E40E59CF26}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1120,9 +1177,9 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1157,7 +1214,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -1171,7 +1227,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1203,7 +1258,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1233,7 +1294,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1277,7 +1344,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1326,7 +1399,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="52" name="Chart 51"/>
+        <xdr:cNvPr id="52" name="Chart 51">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000034000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -1389,7 +1468,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1422,9 +1501,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1457,6 +1553,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1632,18 +1745,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M24"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.54296875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B1" s="2" t="s">
         <v>7</v>
       </c>
@@ -1659,7 +1774,7 @@
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="3">
         <v>2008</v>
@@ -1680,7 +1795,7 @@
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
         <v>3</v>
@@ -1719,7 +1834,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -1760,7 +1875,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -1801,7 +1916,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>1</v>
       </c>
@@ -1842,7 +1957,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B9" s="2" t="s">
         <v>7</v>
       </c>
@@ -1858,7 +1973,7 @@
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B10" s="3">
         <v>2008</v>
       </c>
@@ -1878,7 +1993,7 @@
       <c r="L10" s="3"/>
       <c r="M10" s="3"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B11" s="1" t="s">
         <v>3</v>
       </c>
@@ -1916,166 +2031,130 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>8</v>
       </c>
       <c r="B12">
-        <f ca="1">B13+RANDBETWEEN(20,50)</f>
+        <v>127</v>
+      </c>
+      <c r="C12">
+        <v>91</v>
+      </c>
+      <c r="D12">
+        <v>148</v>
+      </c>
+      <c r="E12">
+        <v>106</v>
+      </c>
+      <c r="F12">
+        <v>136</v>
+      </c>
+      <c r="G12">
+        <v>117</v>
+      </c>
+      <c r="H12">
+        <v>99</v>
+      </c>
+      <c r="I12">
         <v>101</v>
       </c>
-      <c r="C12">
-        <f t="shared" ref="C12:M12" ca="1" si="0">C13+RANDBETWEEN(20,50)</f>
-        <v>102</v>
-      </c>
-      <c r="D12">
-        <f t="shared" ca="1" si="0"/>
-        <v>118</v>
-      </c>
-      <c r="E12">
-        <f t="shared" ca="1" si="0"/>
-        <v>141</v>
-      </c>
-      <c r="F12">
-        <f t="shared" ca="1" si="0"/>
-        <v>128</v>
-      </c>
-      <c r="G12">
-        <f t="shared" ca="1" si="0"/>
-        <v>93</v>
-      </c>
-      <c r="H12">
-        <f t="shared" ca="1" si="0"/>
+      <c r="J12">
+        <v>83</v>
+      </c>
+      <c r="K12">
+        <v>115</v>
+      </c>
+      <c r="L12">
         <v>119</v>
       </c>
-      <c r="I12">
-        <f t="shared" ca="1" si="0"/>
-        <v>111</v>
-      </c>
-      <c r="J12">
-        <f t="shared" ca="1" si="0"/>
-        <v>139</v>
-      </c>
-      <c r="K12">
-        <f t="shared" ca="1" si="0"/>
-        <v>125</v>
-      </c>
-      <c r="L12">
-        <f t="shared" ca="1" si="0"/>
-        <v>90</v>
-      </c>
       <c r="M12">
-        <f t="shared" ca="1" si="0"/>
-        <v>137</v>
+        <v>72</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>9</v>
       </c>
       <c r="B13">
-        <f ca="1">RANDBETWEEN(50,100)</f>
+        <v>84</v>
+      </c>
+      <c r="C13">
         <v>59</v>
       </c>
-      <c r="C13">
-        <f t="shared" ref="C13:M13" ca="1" si="1">RANDBETWEEN(50,100)</f>
-        <v>53</v>
-      </c>
       <c r="D13">
-        <f t="shared" ca="1" si="1"/>
-        <v>78</v>
+        <v>99</v>
       </c>
       <c r="E13">
-        <f t="shared" ca="1" si="1"/>
-        <v>99</v>
+        <v>65</v>
       </c>
       <c r="F13">
-        <f t="shared" ca="1" si="1"/>
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="G13">
-        <f t="shared" ca="1" si="1"/>
-        <v>71</v>
+        <v>91</v>
       </c>
       <c r="H13">
-        <f t="shared" ca="1" si="1"/>
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="I13">
-        <f t="shared" ca="1" si="1"/>
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="J13">
-        <f t="shared" ca="1" si="1"/>
-        <v>100</v>
+        <v>63</v>
       </c>
       <c r="K13">
-        <f t="shared" ca="1" si="1"/>
-        <v>96</v>
+        <v>70</v>
       </c>
       <c r="L13">
-        <f t="shared" ca="1" si="1"/>
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="M13">
-        <f t="shared" ca="1" si="1"/>
-        <v>93</v>
+        <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>10</v>
       </c>
       <c r="B14">
-        <f ca="1">B13-RANDBETWEEN(20,50)</f>
-        <v>23</v>
+        <v>55</v>
       </c>
       <c r="C14">
-        <f t="shared" ref="C14:M14" ca="1" si="2">C13-RANDBETWEEN(20,50)</f>
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="D14">
-        <f t="shared" ca="1" si="2"/>
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="E14">
-        <f t="shared" ca="1" si="2"/>
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="F14">
-        <f t="shared" ca="1" si="2"/>
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="G14">
-        <f t="shared" ca="1" si="2"/>
-        <v>34</v>
+        <v>58</v>
       </c>
       <c r="H14">
-        <f t="shared" ca="1" si="2"/>
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="I14">
-        <f t="shared" ca="1" si="2"/>
         <v>36</v>
       </c>
       <c r="J14">
-        <f t="shared" ca="1" si="2"/>
-        <v>51</v>
+        <v>15</v>
       </c>
       <c r="K14">
-        <f t="shared" ca="1" si="2"/>
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="L14">
-        <f t="shared" ca="1" si="2"/>
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="M14">
-        <f t="shared" ca="1" si="2"/>
-        <v>59</v>
+        <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B17" s="2" t="s">
         <v>7</v>
       </c>
@@ -2091,7 +2170,7 @@
       <c r="L17" s="2"/>
       <c r="M17" s="2"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B18" s="3">
         <v>2008</v>
       </c>
@@ -2111,7 +2190,7 @@
       <c r="L18" s="3"/>
       <c r="M18" s="3"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B19" s="1" t="s">
         <v>3</v>
       </c>
@@ -2149,269 +2228,209 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>11</v>
       </c>
       <c r="B20">
-        <f ca="1">RANDBETWEEN(120,150)</f>
-        <v>130</v>
+        <v>147</v>
       </c>
       <c r="C20">
-        <f ca="1">B23</f>
-        <v>132</v>
+        <v>146</v>
       </c>
       <c r="D20">
-        <f t="shared" ref="D20:M20" ca="1" si="3">C23</f>
-        <v>125</v>
+        <v>206</v>
       </c>
       <c r="E20">
-        <f t="shared" ca="1" si="3"/>
-        <v>141</v>
+        <v>215</v>
       </c>
       <c r="F20">
-        <f t="shared" ca="1" si="3"/>
-        <v>156</v>
+        <v>262</v>
       </c>
       <c r="G20">
-        <f t="shared" ca="1" si="3"/>
+        <v>215</v>
+      </c>
+      <c r="H20">
+        <v>193</v>
+      </c>
+      <c r="I20">
+        <v>159</v>
+      </c>
+      <c r="J20">
+        <v>194</v>
+      </c>
+      <c r="K20">
+        <v>180</v>
+      </c>
+      <c r="L20">
+        <v>154</v>
+      </c>
+      <c r="M20">
         <v>148</v>
       </c>
-      <c r="H20">
-        <f t="shared" ca="1" si="3"/>
-        <v>182</v>
-      </c>
-      <c r="I20">
-        <f t="shared" ca="1" si="3"/>
-        <v>170</v>
-      </c>
-      <c r="J20">
-        <f t="shared" ca="1" si="3"/>
-        <v>173</v>
-      </c>
-      <c r="K20">
-        <f t="shared" ca="1" si="3"/>
-        <v>163</v>
-      </c>
-      <c r="L20">
-        <f t="shared" ca="1" si="3"/>
-        <v>271</v>
-      </c>
-      <c r="M20">
-        <f t="shared" ca="1" si="3"/>
-        <v>276</v>
-      </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>8</v>
       </c>
       <c r="B21">
-        <f ca="1">B20+RANDBETWEEN(20,120)</f>
         <v>204</v>
       </c>
       <c r="C21">
-        <f t="shared" ref="C21:M21" ca="1" si="4">C20+RANDBETWEEN(20,120)</f>
-        <v>197</v>
+        <v>211</v>
       </c>
       <c r="D21">
-        <f t="shared" ca="1" si="4"/>
-        <v>186</v>
+        <v>314</v>
       </c>
       <c r="E21">
-        <f t="shared" ca="1" si="4"/>
-        <v>177</v>
+        <v>283</v>
       </c>
       <c r="F21">
-        <f t="shared" ca="1" si="4"/>
-        <v>211</v>
+        <v>358</v>
       </c>
       <c r="G21">
-        <f t="shared" ca="1" si="4"/>
-        <v>195</v>
+        <v>262</v>
       </c>
       <c r="H21">
-        <f t="shared" ca="1" si="4"/>
-        <v>223</v>
+        <v>295</v>
       </c>
       <c r="I21">
-        <f t="shared" ca="1" si="4"/>
-        <v>275</v>
+        <v>232</v>
       </c>
       <c r="J21">
-        <f t="shared" ca="1" si="4"/>
-        <v>279</v>
+        <v>226</v>
       </c>
       <c r="K21">
-        <f t="shared" ca="1" si="4"/>
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="L21">
-        <f t="shared" ca="1" si="4"/>
-        <v>310</v>
+        <v>180</v>
       </c>
       <c r="M21">
-        <f t="shared" ca="1" si="4"/>
-        <v>305</v>
+        <v>208</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>10</v>
       </c>
       <c r="B22">
-        <f ca="1">B20-RANDBETWEEN(20,50)</f>
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="C22">
-        <f t="shared" ref="C22:M22" ca="1" si="5">C20-RANDBETWEEN(20,50)</f>
-        <v>85</v>
+        <v>121</v>
       </c>
       <c r="D22">
-        <f t="shared" ca="1" si="5"/>
-        <v>87</v>
+        <v>162</v>
       </c>
       <c r="E22">
-        <f t="shared" ca="1" si="5"/>
-        <v>108</v>
+        <v>194</v>
       </c>
       <c r="F22">
-        <f t="shared" ca="1" si="5"/>
-        <v>134</v>
+        <v>214</v>
       </c>
       <c r="G22">
-        <f t="shared" ca="1" si="5"/>
-        <v>124</v>
+        <v>192</v>
       </c>
       <c r="H22">
-        <f t="shared" ca="1" si="5"/>
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="I22">
-        <f t="shared" ca="1" si="5"/>
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="J22">
-        <f t="shared" ca="1" si="5"/>
-        <v>127</v>
+        <v>173</v>
       </c>
       <c r="K22">
-        <f t="shared" ca="1" si="5"/>
-        <v>131</v>
+        <v>148</v>
       </c>
       <c r="L22">
-        <f t="shared" ca="1" si="5"/>
-        <v>249</v>
+        <v>122</v>
       </c>
       <c r="M22">
-        <f t="shared" ca="1" si="5"/>
-        <v>241</v>
+        <v>118</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>12</v>
       </c>
       <c r="B23">
-        <f ca="1">RANDBETWEEN(B22,B21)</f>
-        <v>132</v>
+        <v>146</v>
       </c>
       <c r="C23">
-        <f t="shared" ref="C23:M23" ca="1" si="6">RANDBETWEEN(C22,C21)</f>
-        <v>125</v>
+        <v>206</v>
       </c>
       <c r="D23">
-        <f t="shared" ca="1" si="6"/>
-        <v>141</v>
+        <v>215</v>
       </c>
       <c r="E23">
-        <f t="shared" ca="1" si="6"/>
-        <v>156</v>
+        <v>262</v>
       </c>
       <c r="F23">
-        <f t="shared" ca="1" si="6"/>
+        <v>215</v>
+      </c>
+      <c r="G23">
+        <v>193</v>
+      </c>
+      <c r="H23">
+        <v>159</v>
+      </c>
+      <c r="I23">
+        <v>194</v>
+      </c>
+      <c r="J23">
+        <v>180</v>
+      </c>
+      <c r="K23">
+        <v>154</v>
+      </c>
+      <c r="L23">
         <v>148</v>
       </c>
-      <c r="G23">
-        <f t="shared" ca="1" si="6"/>
-        <v>182</v>
-      </c>
-      <c r="H23">
-        <f t="shared" ca="1" si="6"/>
-        <v>170</v>
-      </c>
-      <c r="I23">
-        <f t="shared" ca="1" si="6"/>
-        <v>173</v>
-      </c>
-      <c r="J23">
-        <f t="shared" ca="1" si="6"/>
-        <v>163</v>
-      </c>
-      <c r="K23">
-        <f t="shared" ca="1" si="6"/>
-        <v>271</v>
-      </c>
-      <c r="L23">
-        <f t="shared" ca="1" si="6"/>
-        <v>276</v>
-      </c>
       <c r="M23">
-        <f t="shared" ca="1" si="6"/>
-        <v>245</v>
+        <v>165</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>13</v>
       </c>
       <c r="B24">
-        <f ca="1">RANDBETWEEN(120,150)</f>
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="C24">
-        <f t="shared" ref="C24:M24" ca="1" si="7">RANDBETWEEN(120,150)</f>
-        <v>138</v>
+        <v>125</v>
       </c>
       <c r="D24">
-        <f t="shared" ca="1" si="7"/>
+        <v>141</v>
+      </c>
+      <c r="E24">
         <v>134</v>
       </c>
-      <c r="E24">
-        <f t="shared" ca="1" si="7"/>
-        <v>143</v>
-      </c>
       <c r="F24">
-        <f t="shared" ca="1" si="7"/>
+        <v>136</v>
+      </c>
+      <c r="G24">
+        <v>124</v>
+      </c>
+      <c r="H24">
+        <v>124</v>
+      </c>
+      <c r="I24">
+        <v>135</v>
+      </c>
+      <c r="J24">
+        <v>131</v>
+      </c>
+      <c r="K24">
+        <v>145</v>
+      </c>
+      <c r="L24">
+        <v>125</v>
+      </c>
+      <c r="M24">
         <v>127</v>
-      </c>
-      <c r="G24">
-        <f t="shared" ca="1" si="7"/>
-        <v>144</v>
-      </c>
-      <c r="H24">
-        <f t="shared" ca="1" si="7"/>
-        <v>148</v>
-      </c>
-      <c r="I24">
-        <f t="shared" ca="1" si="7"/>
-        <v>142</v>
-      </c>
-      <c r="J24">
-        <f t="shared" ca="1" si="7"/>
-        <v>143</v>
-      </c>
-      <c r="K24">
-        <f t="shared" ca="1" si="7"/>
-        <v>143</v>
-      </c>
-      <c r="L24">
-        <f t="shared" ca="1" si="7"/>
-        <v>122</v>
-      </c>
-      <c r="M24">
-        <f t="shared" ca="1" si="7"/>
-        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -2436,7 +2455,39 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
       <x14:sparklineGroups xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-        <x14:sparklineGroup displayEmptyCellsAs="gap">
+        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{00000000-0003-0000-0000-000002000000}">
+          <x14:colorSeries theme="4" tint="-0.499984740745262"/>
+          <x14:colorNegative theme="5"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers theme="4" tint="-0.499984740745262"/>
+          <x14:colorFirst theme="4" tint="0.39997558519241921"/>
+          <x14:colorLast theme="4" tint="0.39997558519241921"/>
+          <x14:colorHigh theme="4"/>
+          <x14:colorLow theme="4"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>Data!B6:M6</xm:f>
+              <xm:sqref>O6</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+        <x14:sparklineGroup type="column" displayEmptyCellsAs="gap" xr2:uid="{00000000-0003-0000-0000-000001000000}">
+          <x14:colorSeries rgb="FFFFC000"/>
+          <x14:colorNegative theme="5"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers theme="4" tint="-0.499984740745262"/>
+          <x14:colorFirst theme="4" tint="0.39997558519241921"/>
+          <x14:colorLast theme="4" tint="0.39997558519241921"/>
+          <x14:colorHigh theme="4"/>
+          <x14:colorLow theme="4"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>Data!B5:M5</xm:f>
+              <xm:sqref>O5</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{00000000-0003-0000-0000-000000000000}">
           <x14:colorSeries theme="4" tint="-0.499984740745262"/>
           <x14:colorNegative theme="5"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -2452,38 +2503,6 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup type="column" displayEmptyCellsAs="gap">
-          <x14:colorSeries rgb="FFFFC000"/>
-          <x14:colorNegative theme="5"/>
-          <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers theme="4" tint="-0.499984740745262"/>
-          <x14:colorFirst theme="4" tint="0.39997558519241921"/>
-          <x14:colorLast theme="4" tint="0.39997558519241921"/>
-          <x14:colorHigh theme="4"/>
-          <x14:colorLow theme="4"/>
-          <x14:sparklines>
-            <x14:sparkline>
-              <xm:f>Data!B5:M5</xm:f>
-              <xm:sqref>O5</xm:sqref>
-            </x14:sparkline>
-          </x14:sparklines>
-        </x14:sparklineGroup>
-        <x14:sparklineGroup displayEmptyCellsAs="gap">
-          <x14:colorSeries theme="4" tint="-0.499984740745262"/>
-          <x14:colorNegative theme="5"/>
-          <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers theme="4" tint="-0.499984740745262"/>
-          <x14:colorFirst theme="4" tint="0.39997558519241921"/>
-          <x14:colorLast theme="4" tint="0.39997558519241921"/>
-          <x14:colorHigh theme="4"/>
-          <x14:colorLow theme="4"/>
-          <x14:sparklines>
-            <x14:sparkline>
-              <xm:f>Data!B6:M6</xm:f>
-              <xm:sqref>O6</xm:sqref>
-            </x14:sparkline>
-          </x14:sparklines>
-        </x14:sparklineGroup>
       </x14:sparklineGroups>
     </ext>
   </extLst>
@@ -2491,14 +2510,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>